<commit_message>
Création de la documentation technique
</commit_message>
<xml_diff>
--- a/Documentation/Planning/planning_reel.xlsx
+++ b/Documentation/Planning/planning_reel.xlsx
@@ -407,7 +407,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -426,19 +426,70 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -453,46 +504,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -831,7 +846,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -860,138 +875,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="40" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="15"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="32"/>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="27">
         <v>42122</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="8">
+      <c r="C2" s="35"/>
+      <c r="D2" s="27">
         <v>42123</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="8">
+      <c r="E2" s="28"/>
+      <c r="F2" s="27">
         <v>42124</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="8">
+      <c r="G2" s="35"/>
+      <c r="H2" s="27">
         <v>42129</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="8">
+      <c r="I2" s="28"/>
+      <c r="J2" s="27">
         <v>42130</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="8">
+      <c r="K2" s="28"/>
+      <c r="L2" s="27">
         <v>42131</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="8">
+      <c r="M2" s="28"/>
+      <c r="N2" s="27">
         <v>42132</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="8">
+      <c r="O2" s="28"/>
+      <c r="P2" s="27">
         <v>42136</v>
       </c>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="8">
+      <c r="Q2" s="28"/>
+      <c r="R2" s="27">
         <v>42137</v>
       </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="8">
+      <c r="S2" s="28"/>
+      <c r="T2" s="27">
         <v>42139</v>
       </c>
-      <c r="U2" s="17"/>
+      <c r="U2" s="29"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="18"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="T3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="U3" s="19" t="s">
+      <c r="U3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="V3" s="1"/>
@@ -999,283 +1014,283 @@
       <c r="X3" s="1"/>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="17"/>
       <c r="J4" s="4"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="28"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="17"/>
       <c r="N4" s="4"/>
       <c r="O4" s="5"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="28"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="17"/>
       <c r="R4" s="4"/>
       <c r="S4" s="5"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="30"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="19"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="4"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="17"/>
       <c r="J5" s="4"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="28"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="17"/>
       <c r="N5" s="4"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="28"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="17"/>
       <c r="R5" s="4"/>
       <c r="S5" s="5"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="30"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="19"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="1:24">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="17"/>
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="28"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="17"/>
       <c r="N6" s="4"/>
       <c r="O6" s="5"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="28"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="17"/>
       <c r="R6" s="4"/>
       <c r="S6" s="5"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="30"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="19"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="2"/>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="28"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17"/>
       <c r="J7" s="4"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="28"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="17"/>
       <c r="N7" s="4"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="28"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="17"/>
       <c r="R7" s="4"/>
       <c r="S7" s="5"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="30"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="19"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="28"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="4"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="28"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="17"/>
       <c r="N8" s="4"/>
       <c r="O8" s="5"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="28"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="17"/>
       <c r="R8" s="4"/>
       <c r="S8" s="5"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="30"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="19"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="28"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="28"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="17"/>
       <c r="N9" s="4"/>
       <c r="O9" s="5"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="28"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="17"/>
       <c r="R9" s="4"/>
       <c r="S9" s="5"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="30"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="19"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="4"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="28"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="17"/>
       <c r="N10" s="4"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="28"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="17"/>
       <c r="R10" s="4"/>
       <c r="S10" s="5"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="30"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="19"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="4"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="28"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17"/>
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="28"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
       <c r="N11" s="4"/>
       <c r="O11" s="5"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="28"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="17"/>
       <c r="R11" s="4"/>
       <c r="S11" s="5"/>
-      <c r="T11" s="29"/>
-      <c r="U11" s="30"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="19"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="4"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="28"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17"/>
       <c r="J12" s="4"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="28"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="17"/>
       <c r="N12" s="4"/>
       <c r="O12" s="5"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="28"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="17"/>
       <c r="R12" s="4"/>
       <c r="S12" s="5"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="30"/>
+      <c r="T12" s="18"/>
+      <c r="U12" s="19"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:24" ht="16" thickBot="1">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="24"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="21"/>
       <c r="L13" s="23"/>
       <c r="M13" s="24"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="24"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="21"/>
       <c r="P13" s="23"/>
       <c r="Q13" s="24"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="24"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="21"/>
       <c r="T13" s="25"/>
       <c r="U13" s="26"/>
       <c r="V13" s="1"/>
@@ -1558,7 +1573,6 @@
     <mergeCell ref="L2:M2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
fin de la gestion de l'avatar et du menu annonce
</commit_message>
<xml_diff>
--- a/Documentation/Planning/planning_reel.xlsx
+++ b/Documentation/Planning/planning_reel.xlsx
@@ -846,7 +846,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F19" sqref="F19:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1137,8 +1137,8 @@
       <c r="C8" s="5"/>
       <c r="D8" s="16"/>
       <c r="E8" s="17"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="2"/>
       <c r="H8" s="16"/>
       <c r="I8" s="17"/>
       <c r="J8" s="4"/>

</xml_diff>

<commit_message>
tous ce qui est en rapport avec les annonces (menu_Annonce, afficher_annonce, modifier_annonce, supprimer_annonce) términer
</commit_message>
<xml_diff>
--- a/Documentation/Planning/planning_reel.xlsx
+++ b/Documentation/Planning/planning_reel.xlsx
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19:F21"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1139,7 +1139,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="3"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="16"/>
+      <c r="H8" s="3"/>
       <c r="I8" s="17"/>
       <c r="J8" s="4"/>
       <c r="K8" s="5"/>
@@ -1168,9 +1168,9 @@
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
       <c r="H9" s="16"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="5"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="16"/>
       <c r="M9" s="17"/>
       <c r="N9" s="4"/>

</xml_diff>

<commit_message>
ajout d'un menu pour activer et désactiver une annonce cote user
ajout d'une valeur supplémentaire "valide" qui vient remplacer l'ancien "active" du coter admin
</commit_message>
<xml_diff>
--- a/Documentation/Planning/planning_reel.xlsx
+++ b/Documentation/Planning/planning_reel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27260" windowHeight="14040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="27260" windowHeight="14040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -846,7 +846,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1171,8 +1171,8 @@
       <c r="I9" s="2"/>
       <c r="J9" s="3"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="17"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="2"/>
       <c r="N9" s="4"/>
       <c r="O9" s="5"/>
       <c r="P9" s="16"/>
@@ -1201,8 +1201,8 @@
       <c r="K10" s="5"/>
       <c r="L10" s="16"/>
       <c r="M10" s="17"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="5"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="2"/>
       <c r="P10" s="16"/>
       <c r="Q10" s="17"/>
       <c r="R10" s="4"/>
@@ -1283,8 +1283,8 @@
       <c r="I13" s="24"/>
       <c r="J13" s="20"/>
       <c r="K13" s="21"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="15"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="24"/>
       <c r="N13" s="20"/>
       <c r="O13" s="21"/>
       <c r="P13" s="23"/>

</xml_diff>